<commit_message>
finalise iconic species list
</commit_message>
<xml_diff>
--- a/circle2016/prep/ICO/spp_ico_list.xlsx
+++ b/circle2016/prep/ICO/spp_ico_list.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22428" windowHeight="6840"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22428" windowHeight="6840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$D$89</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$C$1:$D$1</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="431">
   <si>
     <t>Russia</t>
   </si>
@@ -573,96 +578,24 @@
     <t>razorbills</t>
   </si>
   <si>
-    <t>all all</t>
-  </si>
-  <si>
-    <t>auk</t>
-  </si>
-  <si>
-    <t>Anas acuta</t>
-  </si>
-  <si>
-    <t>pintail</t>
-  </si>
-  <si>
-    <t>Anas crecca</t>
-  </si>
-  <si>
-    <t>common teal</t>
-  </si>
-  <si>
-    <t>Anthus pratensis</t>
-  </si>
-  <si>
-    <t>meadow pipit</t>
-  </si>
-  <si>
-    <t>Carduelis flammea</t>
-  </si>
-  <si>
-    <t>redpolls</t>
-  </si>
-  <si>
-    <t>Charadrius morinellus</t>
-  </si>
-  <si>
-    <t>Eurasian Dotterel</t>
-  </si>
-  <si>
     <t>Chroicocephalus ridibundus</t>
   </si>
   <si>
     <t>hooded gull</t>
   </si>
   <si>
-    <t>Delichon urbicum</t>
-  </si>
-  <si>
-    <t>Common House Martin</t>
-  </si>
-  <si>
-    <t>Gavia immer</t>
-  </si>
-  <si>
-    <t>Great Northern Diver</t>
-  </si>
-  <si>
     <t>Larus argentatus</t>
   </si>
   <si>
     <t>herring gull</t>
   </si>
   <si>
-    <t>Larus canus</t>
-  </si>
-  <si>
-    <t>fiskemåke</t>
-  </si>
-  <si>
     <t>Larus fuscus</t>
   </si>
   <si>
     <t>Lesser Black-backed</t>
   </si>
   <si>
-    <t>Melanitta nigra</t>
-  </si>
-  <si>
-    <t>scoters</t>
-  </si>
-  <si>
-    <t>Oenanthe oenanthe</t>
-  </si>
-  <si>
-    <t>wheatear</t>
-  </si>
-  <si>
-    <t>sturnus vulgaris</t>
-  </si>
-  <si>
-    <t>starling</t>
-  </si>
-  <si>
     <t>Turdus iliacus</t>
   </si>
   <si>
@@ -672,33 +605,18 @@
     <t>Somateria mollissima</t>
   </si>
   <si>
-    <t>eider</t>
-  </si>
-  <si>
     <t>Anser brachyrhynchus</t>
   </si>
   <si>
     <t>Pink-footed Goose</t>
   </si>
   <si>
-    <t>Arenaria inter pres</t>
-  </si>
-  <si>
-    <t>Ruddy Turnstone</t>
-  </si>
-  <si>
     <t>Branta bernicla</t>
   </si>
   <si>
     <t>brent goose</t>
   </si>
   <si>
-    <t>Branta leucopsis</t>
-  </si>
-  <si>
-    <t>barnacle</t>
-  </si>
-  <si>
     <t>Calidris alba</t>
   </si>
   <si>
@@ -711,18 +629,9 @@
     <t>myrsnipe</t>
   </si>
   <si>
-    <t>Calidris canutus</t>
-  </si>
-  <si>
-    <t>red knot</t>
-  </si>
-  <si>
     <t>Cepphus grylle</t>
   </si>
   <si>
-    <t>theist</t>
-  </si>
-  <si>
     <t>Calidris maritima</t>
   </si>
   <si>
@@ -732,21 +641,12 @@
     <t>Charadrius hiaticula</t>
   </si>
   <si>
-    <t>ringed plover</t>
-  </si>
-  <si>
     <t>Clangula hyemalis</t>
   </si>
   <si>
     <t>Long-tailed Ducks</t>
   </si>
   <si>
-    <t>fratercula arctica</t>
-  </si>
-  <si>
-    <t>fairly</t>
-  </si>
-  <si>
     <t>Fulmarus glacialis</t>
   </si>
   <si>
@@ -759,18 +659,9 @@
     <t>Red-throated Diver</t>
   </si>
   <si>
-    <t>lagopus muta</t>
-  </si>
-  <si>
-    <t>Ptarmigan</t>
-  </si>
-  <si>
     <t>Larus hyperboreus</t>
   </si>
   <si>
-    <t>glaucous</t>
-  </si>
-  <si>
     <t>Larus marinus</t>
   </si>
   <si>
@@ -1207,6 +1098,231 @@
   </si>
   <si>
     <t>Phalarop</t>
+  </si>
+  <si>
+    <t>comname</t>
+  </si>
+  <si>
+    <t>sciname</t>
+  </si>
+  <si>
+    <t>ico_gl</t>
+  </si>
+  <si>
+    <t>ico_rgn_id</t>
+  </si>
+  <si>
+    <t>Arctic skua ()</t>
+  </si>
+  <si>
+    <t>Stercocarius parasiticus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arctic tern </t>
+  </si>
+  <si>
+    <t>(Sterna paradisaea)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atlantic puffin </t>
+  </si>
+  <si>
+    <t>(Fratercula arctica)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bearded seal </t>
+  </si>
+  <si>
+    <t>(Erignathus barbatus)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black guillemot </t>
+  </si>
+  <si>
+    <t>(Cepphus grylle)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black-legged kittiwake </t>
+  </si>
+  <si>
+    <t>(Rissa tridactyla)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brünnich’s guillemot </t>
+  </si>
+  <si>
+    <t>(Uria lomvia)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Common guillemot </t>
+  </si>
+  <si>
+    <t>(Uria aalge)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Common minke whale </t>
+  </si>
+  <si>
+    <t>(Balaenoptera acutorostrata)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glaucous gull </t>
+  </si>
+  <si>
+    <t>(Larus hyperboreus)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Great black-backed gull </t>
+  </si>
+  <si>
+    <t>(Larus marinus)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Great northern diver </t>
+  </si>
+  <si>
+    <t>(Gavia immer)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Great skua </t>
+  </si>
+  <si>
+    <t>(Stercorarius skua)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harbour seal </t>
+  </si>
+  <si>
+    <t>(Phoca vitulina)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hooded seal </t>
+  </si>
+  <si>
+    <t>(Cystophora cristata)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Humpback whale </t>
+  </si>
+  <si>
+    <t>(Megaptera novaeangliae)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ivory gull </t>
+  </si>
+  <si>
+    <t>(Pagophila eburnea)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Killer whale </t>
+  </si>
+  <si>
+    <t>(Orcinus orca)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">King eider </t>
+  </si>
+  <si>
+    <t>(Somateria spectabilis)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Little auk </t>
+  </si>
+  <si>
+    <t>(Alle alle)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Narwhal </t>
+  </si>
+  <si>
+    <t>(Monodon monoceros )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern bottlenose whale </t>
+  </si>
+  <si>
+    <t>(Hyperoodon ampullatus)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Polar bear </t>
+  </si>
+  <si>
+    <t>(Ursus maritimus)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pomarine skua </t>
+  </si>
+  <si>
+    <t>(Stercorarius pomarinus)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Razorbill </t>
+  </si>
+  <si>
+    <t>(Alca torda)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ringed seal </t>
+  </si>
+  <si>
+    <t>(Pusa hispida)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ross's gull </t>
+  </si>
+  <si>
+    <t>(Rhodostethia rosea)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sabine's gull </t>
+  </si>
+  <si>
+    <t>(Xema sabini)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sperm whale </t>
+  </si>
+  <si>
+    <t>(Physeter macrocephalus)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">White-beaked dolphin </t>
+  </si>
+  <si>
+    <t>(Lagenorhynchus albirostris)</t>
+  </si>
+  <si>
+    <t>Sterna paradisaea</t>
+  </si>
+  <si>
+    <t>Alle alle</t>
+  </si>
+  <si>
+    <t>Erignathus barbatus</t>
+  </si>
+  <si>
+    <t>Bowhead whale</t>
+  </si>
+  <si>
+    <t>Uria aalge</t>
+  </si>
+  <si>
+    <t>Somateria spectabilis</t>
+  </si>
+  <si>
+    <t>Balaenoptera acutorostrata</t>
+  </si>
+  <si>
+    <t>Stercorarius pomarinus</t>
+  </si>
+  <si>
+    <t>Ringed plover</t>
+  </si>
+  <si>
+    <t>Salmo salar</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -1262,7 +1378,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1270,12 +1386,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDFE2E5"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDFE2E5"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDFE2E5"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDFE2E5"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1292,6 +1423,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1610,8 +1745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M148"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:M65"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45:E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1624,80 +1759,80 @@
         <v>178</v>
       </c>
       <c r="E1" t="s">
-        <v>250</v>
+        <v>212</v>
       </c>
       <c r="G1" t="s">
-        <v>251</v>
+        <v>213</v>
       </c>
       <c r="I1" t="s">
-        <v>337</v>
+        <v>299</v>
       </c>
       <c r="K1" t="s">
-        <v>340</v>
+        <v>302</v>
       </c>
       <c r="M1" t="s">
-        <v>341</v>
+        <v>303</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="27" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>176</v>
+      <c r="C2" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="D2" t="s">
+        <v>361</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>252</v>
+        <v>214</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>253</v>
+        <v>215</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>252</v>
+        <v>214</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>253</v>
+        <v>215</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>338</v>
+        <v>300</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>339</v>
+        <v>301</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>342</v>
+        <v>304</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>342</v>
+        <v>304</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>129</v>
+      <c r="C3" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="D3" t="s">
+        <v>363</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>259</v>
+        <v>221</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>260</v>
+        <v>222</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>259</v>
+        <v>221</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>260</v>
+        <v>222</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>314</v>
+        <v>276</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>176</v>
@@ -1713,99 +1848,99 @@
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>136</v>
+      <c r="C4" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="D4" t="s">
+        <v>365</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>264</v>
+        <v>226</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>167</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>264</v>
+        <v>226</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>167</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>288</v>
+        <v>250</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>142</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>343</v>
+        <v>305</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>343</v>
+        <v>305</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="27" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>180</v>
+      <c r="C5" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5" t="s">
+        <v>367</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>282</v>
+        <v>244</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>283</v>
+        <v>245</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>282</v>
+        <v>244</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>283</v>
+        <v>245</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>264</v>
+        <v>226</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>167</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>344</v>
+        <v>306</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>344</v>
+        <v>306</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>182</v>
+      <c r="C6" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="D6" t="s">
+        <v>369</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>286</v>
+        <v>248</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>287</v>
+        <v>249</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>286</v>
+        <v>248</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>287</v>
+        <v>249</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>345</v>
+        <v>307</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>345</v>
+        <v>307</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="18" x14ac:dyDescent="0.3">
@@ -1813,57 +1948,57 @@
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>185</v>
+        <v>211</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>288</v>
+        <v>250</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>142</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>288</v>
+        <v>250</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>142</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>346</v>
+        <v>308</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>346</v>
+        <v>308</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="27" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>186</v>
+      <c r="C8" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="D8" t="s">
+        <v>371</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>347</v>
+        <v>309</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>347</v>
+        <v>309</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="18" x14ac:dyDescent="0.3">
@@ -1871,19 +2006,19 @@
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>296</v>
+        <v>258</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>147</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>296</v>
+        <v>258</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>147</v>
@@ -1899,23 +2034,23 @@
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>190</v>
+      <c r="C10" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="D10" t="s">
+        <v>373</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>299</v>
+        <v>261</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>300</v>
+        <v>262</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>299</v>
+        <v>261</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>300</v>
+        <v>262</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>146</v>
@@ -1928,23 +2063,23 @@
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>192</v>
+      <c r="C11" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="D11" t="s">
+        <v>375</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>328</v>
+        <v>290</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>304</v>
+        <v>266</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>328</v>
+        <v>290</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>304</v>
+        <v>266</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>150</v>
@@ -1953,24 +2088,24 @@
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="27" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>194</v>
+      <c r="C12" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="D12" t="s">
+        <v>377</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>306</v>
+        <v>268</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>133</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>306</v>
+        <v>268</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>133</v>
@@ -1987,19 +2122,19 @@
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>197</v>
+        <v>130</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>196</v>
+        <v>129</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>307</v>
+        <v>269</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>140</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>307</v>
+        <v>269</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>140</v>
@@ -2011,111 +2146,111 @@
         <v>141</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>198</v>
+      <c r="C14" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="D14" t="s">
+        <v>379</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>309</v>
+        <v>271</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>159</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>309</v>
+        <v>271</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>159</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>348</v>
+        <v>310</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>348</v>
+        <v>310</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="27" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>200</v>
+      <c r="C15" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="D15" t="s">
+        <v>381</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>168</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>168</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>349</v>
+        <v>311</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>349</v>
+        <v>311</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>202</v>
+      <c r="C16" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="D16" t="s">
+        <v>383</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K16" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="G16" s="1" t="s">
+      <c r="M16" s="1" t="s">
         <v>312</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>204</v>
+      <c r="C17" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="D17" t="s">
+        <v>385</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>314</v>
+        <v>276</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>176</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>314</v>
+        <v>276</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>176</v>
@@ -2131,29 +2266,29 @@
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>206</v>
+      <c r="C18" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="D18" t="s">
+        <v>387</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>316</v>
+        <v>278</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>317</v>
+        <v>279</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>316</v>
+        <v>278</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>317</v>
+        <v>279</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>351</v>
+        <v>313</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>351</v>
+        <v>313</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="18" x14ac:dyDescent="0.3">
@@ -2161,202 +2296,202 @@
         <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>320</v>
+        <v>282</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>321</v>
+        <v>283</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>320</v>
+        <v>282</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>321</v>
+        <v>283</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>352</v>
+        <v>314</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="18" x14ac:dyDescent="0.3">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="27" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>211</v>
+        <v>183</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>210</v>
+        <v>182</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>322</v>
+        <v>284</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>323</v>
+        <v>285</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>322</v>
+        <v>284</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>323</v>
+        <v>285</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>353</v>
+        <v>315</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>353</v>
+        <v>315</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>212</v>
+      <c r="C21" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="D21" t="s">
+        <v>389</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>324</v>
+        <v>286</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>325</v>
+        <v>287</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>324</v>
+        <v>286</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>325</v>
+        <v>287</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>354</v>
+        <v>316</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>354</v>
+        <v>316</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>214</v>
+      <c r="C22" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="D22" t="s">
+        <v>391</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>326</v>
+        <v>288</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>327</v>
+        <v>289</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>326</v>
+        <v>288</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>327</v>
+        <v>289</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>355</v>
+        <v>317</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="27" x14ac:dyDescent="0.3">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>216</v>
+      <c r="C23" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="D23" t="s">
+        <v>393</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>329</v>
+        <v>291</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>330</v>
+        <v>292</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>329</v>
+        <v>291</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>330</v>
+        <v>292</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>356</v>
+        <v>318</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>356</v>
+        <v>318</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>218</v>
+      <c r="C24" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="D24" t="s">
+        <v>395</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>331</v>
+        <v>293</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>332</v>
+        <v>294</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>333</v>
+        <v>295</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>334</v>
+        <v>296</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>357</v>
+        <v>319</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>357</v>
+        <v>319</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>220</v>
+      <c r="C25" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="D25" t="s">
+        <v>397</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>333</v>
+        <v>295</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>334</v>
+        <v>296</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>335</v>
+        <v>297</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>336</v>
+        <v>298</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>217</v>
+        <v>192</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>217</v>
+        <v>192</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="27" x14ac:dyDescent="0.3">
@@ -2364,39 +2499,39 @@
         <v>25</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>223</v>
+        <v>187</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>222</v>
+        <v>186</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>335</v>
+        <v>297</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>336</v>
+        <v>298</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>358</v>
+        <v>320</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>358</v>
+        <v>320</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>224</v>
+      <c r="C27" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="D27" t="s">
+        <v>399</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>359</v>
+        <v>321</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>359</v>
+        <v>321</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="18" x14ac:dyDescent="0.3">
@@ -2404,10 +2539,10 @@
         <v>27</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>227</v>
+        <v>204</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>226</v>
+        <v>203</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>21</v>
@@ -2421,103 +2556,103 @@
         <v>28</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>229</v>
+        <v>198</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>228</v>
+        <v>197</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>360</v>
+        <v>322</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>360</v>
+        <v>322</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>230</v>
+      <c r="C30" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="D30" t="s">
+        <v>401</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>361</v>
+        <v>323</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>361</v>
+        <v>323</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>232</v>
+      <c r="C31" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="D31" t="s">
+        <v>403</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="K31" s="1" t="s">
-        <v>362</v>
+        <v>324</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="18" x14ac:dyDescent="0.3">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="27" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>235</v>
+        <v>192</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>234</v>
+        <v>191</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>363</v>
+        <v>325</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>363</v>
+        <v>325</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>236</v>
+      <c r="C33" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="D33" t="s">
+        <v>405</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>364</v>
+        <v>326</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>364</v>
+        <v>326</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>238</v>
+      <c r="C34" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="D34" t="s">
+        <v>407</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>365</v>
+        <v>327</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>365</v>
+        <v>327</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="18" x14ac:dyDescent="0.3">
@@ -2525,33 +2660,33 @@
         <v>34</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>241</v>
+        <v>201</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>240</v>
+        <v>200</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>366</v>
+        <v>328</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>366</v>
+        <v>328</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>242</v>
+      <c r="C36" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="D36" t="s">
+        <v>409</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>367</v>
+        <v>329</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>367</v>
+        <v>329</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="27" x14ac:dyDescent="0.3">
@@ -2559,16 +2694,16 @@
         <v>36</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>245</v>
+        <v>181</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>244</v>
+        <v>180</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>368</v>
+        <v>330</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>368</v>
+        <v>330</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="18" x14ac:dyDescent="0.3">
@@ -2576,16 +2711,16 @@
         <v>37</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>247</v>
+        <v>208</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>246</v>
+        <v>207</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>369</v>
+        <v>331</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>369</v>
+        <v>331</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="18" x14ac:dyDescent="0.3">
@@ -2593,82 +2728,118 @@
         <v>38</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>249</v>
+        <v>189</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>248</v>
+        <v>188</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>370</v>
+        <v>332</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>370</v>
+        <v>332</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="C40" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="D40" t="s">
+        <v>411</v>
+      </c>
       <c r="K40" s="1" t="s">
-        <v>371</v>
+        <v>333</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>371</v>
+        <v>333</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="C41" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="D41" t="s">
+        <v>413</v>
+      </c>
       <c r="K41" s="1" t="s">
-        <v>372</v>
+        <v>334</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>372</v>
+        <v>334</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="C42" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="D42" t="s">
+        <v>415</v>
+      </c>
       <c r="K42" s="1" t="s">
-        <v>373</v>
+        <v>335</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>373</v>
+        <v>335</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="C43" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="D43" t="s">
+        <v>417</v>
+      </c>
       <c r="K43" s="1" t="s">
-        <v>374</v>
+        <v>336</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>374</v>
+        <v>336</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="C44" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="K44" s="1" t="s">
-        <v>375</v>
+        <v>337</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>375</v>
+        <v>337</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="27" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="C45" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="D45" t="s">
+        <v>419</v>
+      </c>
       <c r="K45" s="1" t="s">
-        <v>376</v>
+        <v>338</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>376</v>
+        <v>338</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="18" x14ac:dyDescent="0.3">
@@ -2687,10 +2858,10 @@
         <v>46</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>377</v>
+        <v>339</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>377</v>
+        <v>339</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="18" x14ac:dyDescent="0.3">
@@ -2698,10 +2869,10 @@
         <v>47</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>378</v>
+        <v>340</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>378</v>
+        <v>340</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
@@ -2709,10 +2880,10 @@
         <v>48</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>379</v>
+        <v>341</v>
       </c>
       <c r="M49" s="1" t="s">
-        <v>379</v>
+        <v>341</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
@@ -2720,10 +2891,10 @@
         <v>49</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>380</v>
+        <v>342</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>380</v>
+        <v>342</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="18" x14ac:dyDescent="0.3">
@@ -2731,10 +2902,10 @@
         <v>50</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>381</v>
+        <v>343</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>381</v>
+        <v>343</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="18" x14ac:dyDescent="0.3">
@@ -2742,10 +2913,10 @@
         <v>51</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>382</v>
+        <v>344</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>382</v>
+        <v>344</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="18" x14ac:dyDescent="0.3">
@@ -2753,10 +2924,10 @@
         <v>52</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>383</v>
+        <v>345</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>383</v>
+        <v>345</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="18" x14ac:dyDescent="0.3">
@@ -2764,10 +2935,10 @@
         <v>53</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>384</v>
+        <v>346</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>384</v>
+        <v>346</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="18" x14ac:dyDescent="0.3">
@@ -2775,10 +2946,10 @@
         <v>54</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>385</v>
+        <v>347</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>385</v>
+        <v>347</v>
       </c>
     </row>
     <row r="56" spans="1:13" ht="27" x14ac:dyDescent="0.3">
@@ -2797,10 +2968,10 @@
         <v>56</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>386</v>
+        <v>348</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>386</v>
+        <v>348</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.3">
@@ -2808,10 +2979,10 @@
         <v>57</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>387</v>
+        <v>349</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>387</v>
+        <v>349</v>
       </c>
     </row>
     <row r="59" spans="1:13" ht="18" x14ac:dyDescent="0.3">
@@ -2819,10 +2990,10 @@
         <v>58</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>388</v>
+        <v>350</v>
       </c>
       <c r="M59" s="1" t="s">
-        <v>388</v>
+        <v>350</v>
       </c>
     </row>
     <row r="60" spans="1:13" ht="18" x14ac:dyDescent="0.3">
@@ -2830,10 +3001,10 @@
         <v>59</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>389</v>
+        <v>351</v>
       </c>
       <c r="M60" s="1" t="s">
-        <v>389</v>
+        <v>351</v>
       </c>
     </row>
     <row r="61" spans="1:13" ht="18" x14ac:dyDescent="0.3">
@@ -2852,10 +3023,10 @@
         <v>61</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>390</v>
+        <v>352</v>
       </c>
       <c r="M62" s="1" t="s">
-        <v>390</v>
+        <v>352</v>
       </c>
     </row>
     <row r="63" spans="1:13" ht="18" x14ac:dyDescent="0.3">
@@ -2863,10 +3034,10 @@
         <v>62</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>391</v>
+        <v>353</v>
       </c>
       <c r="M63" s="1" t="s">
-        <v>391</v>
+        <v>353</v>
       </c>
     </row>
     <row r="64" spans="1:13" ht="18" x14ac:dyDescent="0.3">
@@ -2874,10 +3045,10 @@
         <v>63</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>392</v>
+        <v>354</v>
       </c>
       <c r="M64" s="1" t="s">
-        <v>392</v>
+        <v>354</v>
       </c>
     </row>
     <row r="65" spans="1:13" ht="18" x14ac:dyDescent="0.3">
@@ -2885,10 +3056,10 @@
         <v>64</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>393</v>
+        <v>355</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>393</v>
+        <v>355</v>
       </c>
     </row>
     <row r="66" spans="1:13" ht="18" x14ac:dyDescent="0.3">
@@ -3379,15 +3550,1466 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="C1:D1">
+    <sortState ref="C2:D65">
+      <sortCondition ref="C1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D118"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>420</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>420</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>420</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>420</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>420</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>422</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>422</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>422</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>422</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>422</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C25" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="8" t="s">
+        <v>423</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C29" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>424</v>
+      </c>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>424</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>424</v>
+      </c>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="C36" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C57" s="8"/>
+      <c r="D57" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C59" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="C61" s="8"/>
+      <c r="D61" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="C62" s="8"/>
+      <c r="D62" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="C63" s="8"/>
+      <c r="D63" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="C64" s="8"/>
+      <c r="D64" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C65" s="8"/>
+      <c r="D65" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C66" s="8"/>
+      <c r="D66" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
+    </row>
+    <row r="70" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>425</v>
+      </c>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>425</v>
+      </c>
+      <c r="C71" s="8"/>
+      <c r="D71" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>425</v>
+      </c>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>421</v>
+      </c>
+      <c r="C73" s="8"/>
+      <c r="D73" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>421</v>
+      </c>
+      <c r="C74" s="8"/>
+      <c r="D74" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>421</v>
+      </c>
+      <c r="C75" s="8"/>
+      <c r="D75" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>426</v>
+      </c>
+      <c r="C76" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D76" s="8" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C77" s="8"/>
+      <c r="D77" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C78" s="8"/>
+      <c r="D78" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C79" s="8"/>
+      <c r="D79" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C80" s="8"/>
+      <c r="D80" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C81" s="8"/>
+      <c r="D81" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C82" s="8"/>
+      <c r="D82" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C83" s="8"/>
+      <c r="D83" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C84" s="8"/>
+      <c r="D84" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C85" s="8"/>
+      <c r="D85" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C86" s="8"/>
+      <c r="D86" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C87" s="8"/>
+      <c r="D87" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A88" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C88" s="8"/>
+      <c r="D88" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A89" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C89" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D89" s="8" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A90" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="C90" s="8"/>
+      <c r="D90" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A91" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="C91" s="8"/>
+      <c r="D91" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A92" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="B92" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="C92" s="8"/>
+      <c r="D92" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A93" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="C93" s="8"/>
+      <c r="D93" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A94" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="C94" s="8"/>
+      <c r="D94" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A95" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="C95" s="8"/>
+      <c r="D95" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A96" s="8" t="s">
+        <v>428</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="C96" s="8"/>
+      <c r="D96" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="C97" s="8"/>
+      <c r="D97" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A98" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="B98" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="C98" s="8"/>
+      <c r="D98" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A99" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="C99" s="8"/>
+      <c r="D99" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A100" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="B100" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="C100" s="8"/>
+      <c r="D100" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A101" s="8" t="s">
+        <v>306</v>
+      </c>
+      <c r="B101" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="C101" s="8"/>
+      <c r="D101" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A102" s="8" t="s">
+        <v>306</v>
+      </c>
+      <c r="B102" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="C102" s="8"/>
+      <c r="D102" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A103" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="B103" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="C103" s="8"/>
+      <c r="D103" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A104" s="8" t="s">
+        <v>346</v>
+      </c>
+      <c r="B104" s="8" t="s">
+        <v>429</v>
+      </c>
+      <c r="C104" s="8"/>
+      <c r="D104" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A105" s="8" t="s">
+        <v>346</v>
+      </c>
+      <c r="B105" s="8" t="s">
+        <v>429</v>
+      </c>
+      <c r="C105" s="8"/>
+      <c r="D105" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A106" s="8" t="s">
+        <v>346</v>
+      </c>
+      <c r="B106" s="8" t="s">
+        <v>429</v>
+      </c>
+      <c r="C106" s="8"/>
+      <c r="D106" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A107" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="B107" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="C107" s="8"/>
+      <c r="D107" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A108" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="B108" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="C108" s="8"/>
+      <c r="D108" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A109" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="B109" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="C109" s="8"/>
+      <c r="D109" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A110" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="B110" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C110" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D110" s="8" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A111" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B111" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C111" s="8"/>
+      <c r="D111" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A112" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B112" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C112" s="8"/>
+      <c r="D112" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A113" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B113" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C113" s="8"/>
+      <c r="D113" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A114" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B114" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C114" s="8"/>
+      <c r="D114" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A115" s="8" t="s">
+        <v>418</v>
+      </c>
+      <c r="B115" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="C115" s="8"/>
+      <c r="D115" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A116" s="8" t="s">
+        <v>418</v>
+      </c>
+      <c r="B116" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="C116" s="8"/>
+      <c r="D116" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A117" s="8" t="s">
+        <v>418</v>
+      </c>
+      <c r="B117" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="C117" s="8"/>
+      <c r="D117" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A118" s="8" t="s">
+        <v>418</v>
+      </c>
+      <c r="B118" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="C118" s="8"/>
+      <c r="D118" s="8">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B1" sqref="A1:B29"/>
     </sheetView>
   </sheetViews>
@@ -3395,689 +5017,689 @@
   <sheetData>
     <row r="1" spans="1:8" ht="153" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>252</v>
+        <v>214</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>253</v>
+        <v>215</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4" t="s">
-        <v>254</v>
+        <v>216</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>255</v>
+        <v>217</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>256</v>
+        <v>218</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>257</v>
+        <v>219</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>258</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>259</v>
+        <v>221</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>260</v>
+        <v>222</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
-        <v>261</v>
+        <v>223</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>262</v>
+        <v>224</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>256</v>
+        <v>218</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>263</v>
+        <v>225</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>256</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>264</v>
+        <v>226</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>167</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>265</v>
+        <v>227</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>254</v>
+        <v>216</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>266</v>
+        <v>228</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>267</v>
+        <v>229</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>257</v>
+        <v>219</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>258</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>264</v>
+        <v>226</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>167</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>268</v>
+        <v>230</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>254</v>
+        <v>216</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>269</v>
+        <v>231</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>270</v>
+        <v>232</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>257</v>
+        <v>219</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>258</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="51" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>264</v>
+        <v>226</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>167</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>271</v>
+        <v>233</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>254</v>
+        <v>216</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>266</v>
+        <v>228</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>256</v>
+        <v>218</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>257</v>
+        <v>219</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>258</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="51" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>264</v>
+        <v>226</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>167</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>272</v>
+        <v>234</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>254</v>
+        <v>216</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>273</v>
+        <v>235</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>270</v>
+        <v>232</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>257</v>
+        <v>219</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>258</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>264</v>
+        <v>226</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>167</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>274</v>
+        <v>236</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>254</v>
+        <v>216</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>275</v>
+        <v>237</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>276</v>
+        <v>238</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8" ht="71.400000000000006" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>264</v>
+        <v>226</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>167</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>277</v>
+        <v>239</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>254</v>
+        <v>216</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>278</v>
+        <v>240</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>256</v>
+        <v>218</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>257</v>
+        <v>219</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>258</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>264</v>
+        <v>226</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>167</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>254</v>
+        <v>216</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>266</v>
+        <v>228</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>280</v>
+        <v>242</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>281</v>
+        <v>243</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>270</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>282</v>
+        <v>244</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>283</v>
+        <v>245</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6" t="s">
-        <v>261</v>
+        <v>223</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>179</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>284</v>
+        <v>246</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>285</v>
+        <v>247</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>256</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>286</v>
+        <v>248</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>287</v>
+        <v>249</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
-        <v>261</v>
+        <v>223</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>179</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>284</v>
+        <v>246</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>285</v>
+        <v>247</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>256</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>288</v>
+        <v>250</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>142</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>289</v>
+        <v>251</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>254</v>
+        <v>216</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>179</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>256</v>
+        <v>218</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>263</v>
+        <v>225</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>256</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>288</v>
+        <v>250</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>142</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>290</v>
+        <v>252</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>254</v>
+        <v>216</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>179</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>280</v>
+        <v>242</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>281</v>
+        <v>243</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>270</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="51" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>288</v>
+        <v>250</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>142</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>254</v>
+        <v>216</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>179</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>256</v>
+        <v>218</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>257</v>
+        <v>219</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>258</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>261</v>
+        <v>223</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>295</v>
+        <v>257</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>276</v>
+        <v>238</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>296</v>
+        <v>258</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>147</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>297</v>
+        <v>259</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>254</v>
+        <v>216</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>298</v>
+        <v>260</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>256</v>
+        <v>218</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>263</v>
+        <v>225</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>256</v>
+        <v>218</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>299</v>
+        <v>261</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>300</v>
+        <v>262</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>301</v>
+        <v>263</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>254</v>
+        <v>216</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>302</v>
+        <v>264</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>256</v>
+        <v>218</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>263</v>
+        <v>225</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>256</v>
+        <v>218</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="183.6" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>303</v>
+        <v>265</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>304</v>
+        <v>266</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6" t="s">
-        <v>254</v>
+        <v>216</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>305</v>
+        <v>267</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>276</v>
+        <v>238</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:8" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>306</v>
+        <v>268</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>133</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4" t="s">
-        <v>254</v>
+        <v>216</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>262</v>
+        <v>224</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>276</v>
+        <v>238</v>
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
     <row r="20" spans="1:8" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>307</v>
+        <v>269</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>140</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>308</v>
+        <v>270</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>254</v>
+        <v>216</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>262</v>
+        <v>224</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>276</v>
+        <v>238</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>285</v>
+        <v>247</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>256</v>
+        <v>218</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="51" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>309</v>
+        <v>271</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>159</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>310</v>
+        <v>272</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>254</v>
+        <v>216</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>262</v>
+        <v>224</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>256</v>
+        <v>218</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>257</v>
+        <v>219</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>258</v>
+        <v>220</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>168</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6" t="s">
-        <v>254</v>
+        <v>216</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>179</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>256</v>
+        <v>218</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>257</v>
+        <v>219</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>258</v>
+        <v>220</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>312</v>
+        <v>274</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>313</v>
+        <v>275</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4" t="s">
-        <v>261</v>
+        <v>223</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>262</v>
+        <v>224</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>267</v>
+        <v>229</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>263</v>
+        <v>225</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>267</v>
+        <v>229</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="122.4" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>314</v>
+        <v>276</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>176</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6" t="s">
-        <v>254</v>
+        <v>216</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>315</v>
+        <v>277</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>256</v>
+        <v>218</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>263</v>
+        <v>225</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>256</v>
+        <v>218</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="285.60000000000002" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>316</v>
+        <v>278</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>317</v>
+        <v>279</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4" t="s">
-        <v>318</v>
+        <v>280</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>319</v>
+        <v>281</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>256</v>
+        <v>218</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>257</v>
+        <v>219</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>258</v>
+        <v>220</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>320</v>
+        <v>282</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>321</v>
+        <v>283</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6" t="s">
-        <v>254</v>
+        <v>216</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>262</v>
+        <v>224</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>276</v>
+        <v>238</v>
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
     </row>
     <row r="27" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>322</v>
+        <v>284</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>323</v>
+        <v>285</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4" t="s">
-        <v>261</v>
+        <v>223</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>262</v>
+        <v>224</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>270</v>
+        <v>232</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>257</v>
+        <v>219</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>258</v>
+        <v>220</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>324</v>
+        <v>286</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>325</v>
+        <v>287</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6" t="s">
-        <v>261</v>
+        <v>223</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>262</v>
+        <v>224</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>267</v>
+        <v>229</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>263</v>
+        <v>225</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>267</v>
+        <v>229</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>326</v>
+        <v>288</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>

</xml_diff>